<commit_message>
In red identical versions removed from input_files_for_db. In red kept.
</commit_message>
<xml_diff>
--- a/data/lrp_data_legend.xlsx
+++ b/data/lrp_data_legend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diandra/rlp_meta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C3FF89-0660-D04C-BB9B-11D0BA9F5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40AFDE3-A7FA-064E-8453-6E769A8DCD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{5B21510A-2186-C449-9A1B-808F36C921CB}"/>
+    <workbookView xWindow="14220" yWindow="3200" windowWidth="20340" windowHeight="17440" xr2:uid="{5B21510A-2186-C449-9A1B-808F36C921CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
     <t>https://string-db.org/cgi/download?sessionId=bGZ5zi4vdyus</t>
   </si>
   <si>
-    <t>tot=25 + 2</t>
+    <t>tot=20 + 2</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -284,6 +290,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D106CA5-723D-F641-B630-1737F9CADC3E}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,7 +751,7 @@
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -815,7 +823,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -852,7 +860,7 @@
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2"/>
@@ -871,7 +879,7 @@
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -894,7 +902,7 @@
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="2"/>
@@ -945,7 +953,7 @@
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="2"/>

</xml_diff>